<commit_message>
adding super secerate stuff
</commit_message>
<xml_diff>
--- a/analyse tabel.xlsx
+++ b/analyse tabel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sijmen\Documents\SubSet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="6675" windowHeight="7230"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="6672" windowHeight="7236"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="103">
   <si>
     <t>addCardToScreen(int cardID, int x, int y)</t>
   </si>
@@ -24,9 +29,6 @@
     <t>backToMenu() </t>
   </si>
   <si>
-    <t>cardClickedAction(int id) </t>
-  </si>
-  <si>
     <t>cardDragAction() </t>
   </si>
   <si>
@@ -111,18 +113,12 @@
     <t>saveAndQuit() </t>
   </si>
   <si>
-    <t>saveGame() </t>
-  </si>
-  <si>
     <t>showAboutScreen() </t>
   </si>
   <si>
     <t>showScoreScreen()</t>
   </si>
   <si>
-    <t>shuffleStack(processing.data.StringList in) </t>
-  </si>
-  <si>
     <t>startGame(boolean original) </t>
   </si>
   <si>
@@ -147,18 +143,12 @@
     <t>isSameOrDiff(StringtoCheck) </t>
   </si>
   <si>
-    <t>addSelectedCard(Stringcard) </t>
-  </si>
-  <si>
     <t>loadScoreBoard(Stringfile) </t>
   </si>
   <si>
     <t>addButton(Stringnaam, int id, int menu, int x, int y, int wid, int hei, int bgCol, int fgCol)</t>
   </si>
   <si>
-    <t>removeSelectedCard(Stringcard) </t>
-  </si>
-  <si>
     <t xml:space="preserve"> boolean</t>
   </si>
   <si>
@@ -222,9 +212,6 @@
     <t>handInSet() </t>
   </si>
   <si>
-    <t>Wat is de functionaliteit?</t>
-  </si>
-  <si>
     <t>Teken alle zichtbare knoppen op een schem.</t>
   </si>
   <si>
@@ -250,6 +237,99 @@
   </si>
   <si>
     <t>Deze functie wordt aangeroepen als op de knop "Score Board" gedrukt wordt.</t>
+  </si>
+  <si>
+    <t>Voegt een nieuwe kaart toe met het gegeven id nummer. De x en y zijn de kaart x en y. Kaart 1 heeft 0,0; kaart 2 heeft 1,0 enzovoort.</t>
+  </si>
+  <si>
+    <t>addSelectedCard(String card) </t>
+  </si>
+  <si>
+    <t>Voegt een bepaalde kaart toe aan het selectedCards array. Deze functie geeft de locatie (0-2) terug waar de kaart is opgeslagen. Als er geen plek was, wordt -1 terug gegeven.</t>
+  </si>
+  <si>
+    <t>Kijkt of een van de kaarten verschoven moet worden. Deze functie wordt aangeroepen als mouseDragged event is gebeurt.</t>
+  </si>
+  <si>
+    <t>Wordt aangeroepen als de muis is ingedrukt boven een kaart. Deze functie start het draggen van de kaart.</t>
+  </si>
+  <si>
+    <t>Wat moet er met de kaarten gebeuren als de muis is los gelaten? Moet er worden gestopt met schuiven? Moet een kaart naar linksonder worden verplaats? Dit zijn taken van deze functie.</t>
+  </si>
+  <si>
+    <t>Tekent een bepaalde kaart. Welke kaart getekent moet worden wordt aangegeven door de dataLocation.</t>
+  </si>
+  <si>
+    <t>Maakt een stapel kaarten. Met de simple boolena wordt aangegeven of de simpele versie met 29 of de moeiljijke versie met 81 kaarten gemaaakt meot worden.</t>
+  </si>
+  <si>
+    <t>Geeft een Rectangle met x, y, breedte en hoogte met de standaard locatie van een kaart op het schem. De x en y zijn dus niet een x en y op het schem maar een row en column in de kaarten op het schem.</t>
+  </si>
+  <si>
+    <t>Geeft een Rectangle met x, y, breedte en hoogte met de seleted hokjes links onder op het schem. Het nr is 0,1 of 2. Deze geeft aan om welk hokje het gaat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maakt een nieuwe kaart door middel van een kleur, vorm, aantal en achtergrond. Al deze getallen zijn 1, 2 of 3. Met uitzondering van background: deze kan ook 4 zijn. </t>
+  </si>
+  <si>
+    <t>Rangschik alle kaarten op het schem naar hun standaard locatie.</t>
+  </si>
+  <si>
+    <t>Wat is de functionaliteit/argumenten?</t>
+  </si>
+  <si>
+    <t>removeSelectedCard(String card) </t>
+  </si>
+  <si>
+    <t>Verwijdert een van de geselecteerde kaarten. De String card geeft aan om welke kaart het gaat.</t>
+  </si>
+  <si>
+    <t>shuffleStack(StringList in) </t>
+  </si>
+  <si>
+    <t>Geef een Lijst met kaarten, en deze functie zal de kaarten schudden.</t>
+  </si>
+  <si>
+    <t>Deze functie tekent het about scherm</t>
+  </si>
+  <si>
+    <t>Deze functie tekent het menu.</t>
+  </si>
+  <si>
+    <t>Deze functie tekent het score bord.</t>
+  </si>
+  <si>
+    <t>Deze functie roept de juiste teken functie aan.</t>
+  </si>
+  <si>
+    <t>Deze functie tekent de game.</t>
+  </si>
+  <si>
+    <t>Deze functie selecteerd twee kaarten die samen met een derde een set vormen. Deze derde ligt ook op het schem.</t>
+  </si>
+  <si>
+    <t>Deze functie stopt het spel en verwijst terug naar het score bord.</t>
+  </si>
+  <si>
+    <t>Als de knop "Han In" linksonder in het game schem opgelicht is omdat er goede set geselecteerd is, dan kan je met deze knop de kaarten inleveren. Deze functie levert de functinalieteit voor deze actie.</t>
+  </si>
+  <si>
+    <t>Deze functie is een baas. Hij kan doormiddel van slimmigheid contoroleren of een aantal kaarten wel of niet een set zijn. Hij is geschikt van 2 tm oneindig aantal kaarten.</t>
+  </si>
+  <si>
+    <t>Deze functie laad een opgeslagen spel vanuit de harde schijf.</t>
+  </si>
+  <si>
+    <t>Hij slaat de huidigge game op en gaat terug naar het menu.</t>
+  </si>
+  <si>
+    <t>Hij slaat de huidigge game op.</t>
+  </si>
+  <si>
+    <t>saveGame(String file) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Er wordt een nieuwe spelletje gestart. </t>
   </si>
 </sst>
 </file>
@@ -306,6 +386,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -353,7 +436,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +471,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,599 +680,666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="78.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="1" max="1" width="78.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="81.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" t="s">
-        <v>51</v>
-      </c>
       <c r="C45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1209,7 +1359,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1221,7 +1371,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
noog meeer analyse. Ik wordt er helemaal gek van.
</commit_message>
<xml_diff>
--- a/analyse tabel.xlsx
+++ b/analyse tabel.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Functies" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functies!$A$1:$D$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Functies!$A$1:$D$58</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -229,9 +229,6 @@
     <t>removeSelectedCard(int[] button) </t>
   </si>
   <si>
-    <t>shuffleStack(processing.data.StringList in) </t>
-  </si>
-  <si>
     <t>startGame(boolean original)</t>
   </si>
   <si>
@@ -431,6 +428,9 @@
   </si>
   <si>
     <t>addButton(String naam, int id, int scherm, int x, int y, int wid, int hei, int bgCol, int fgCol)</t>
+  </si>
+  <si>
+    <t>shuffleStack(StringList in) </t>
   </si>
 </sst>
 </file>
@@ -454,12 +454,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -474,10 +480,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -786,15 +795,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="135.7109375" customWidth="1"/>
+    <col min="4" max="4" width="201.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -812,86 +821,86 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -903,7 +912,7 @@
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
         <v>38</v>
@@ -914,13 +923,13 @@
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,7 +940,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -942,13 +951,13 @@
         <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -959,10 +968,10 @@
         <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,10 +982,10 @@
         <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -987,23 +996,23 @@
         <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1015,7 +1024,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
@@ -1026,13 +1035,13 @@
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1040,13 +1049,13 @@
         <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,24 +1066,24 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" t="s">
-        <v>113</v>
+      <c r="B20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1082,26 +1091,26 @@
         <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1113,93 +1122,93 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="A24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" t="s">
-        <v>106</v>
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1211,10 +1220,10 @@
         <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1225,7 +1234,7 @@
         <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
         <v>53</v>
@@ -1233,58 +1242,58 @@
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
         <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1295,66 +1304,66 @@
         <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" t="s">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
         <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,10 +1374,10 @@
         <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1379,94 +1388,94 @@
         <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="A43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" t="s">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" t="s">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" t="s">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1477,10 +1486,10 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1488,13 +1497,13 @@
         <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1505,10 +1514,10 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1519,7 +1528,7 @@
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -1533,10 +1542,10 @@
         <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1544,13 +1553,13 @@
         <v>64</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1558,41 +1567,41 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56" t="s">
-        <v>85</v>
-      </c>
-      <c r="D56" t="s">
-        <v>112</v>
+      <c r="A56" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1600,34 +1609,33 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
         <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D59">
-    <sortState ref="A2:D59">
-      <sortCondition ref="C2:C66"/>
-      <sortCondition ref="A2:A66"/>
+  <autoFilter ref="A1:D58">
+    <sortState ref="A2:D60">
+      <sortCondition ref="C1:C59"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:D79">

</xml_diff>

<commit_message>
nu gaat het weer een beetje beter met analyseren.
</commit_message>
<xml_diff>
--- a/analyse tabel.xlsx
+++ b/analyse tabel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sijmen\Documents\SubSet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="6675" windowHeight="7230"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="6672" windowHeight="7236"/>
   </bookViews>
   <sheets>
     <sheet name="Functies" sheetId="2" r:id="rId1"/>
@@ -547,7 +552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,7 +587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,20 +798,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="201.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="201.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -820,7 +825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>136</v>
       </c>
@@ -834,7 +839,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
@@ -848,7 +853,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -862,7 +867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -876,7 +881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -890,7 +895,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -904,21 +909,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -932,7 +937,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -946,7 +951,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -960,7 +965,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -974,7 +979,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -988,7 +993,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>92</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1044,7 +1049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1058,7 +1063,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1077,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1086,7 +1091,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1100,7 +1105,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -1114,7 +1119,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>137</v>
       </c>
@@ -1142,7 +1147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1156,7 +1161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1175,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -1184,7 +1189,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -1212,7 +1217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1240,7 +1245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1254,7 +1259,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1268,7 +1273,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1282,7 +1287,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1296,7 +1301,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1310,7 +1315,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>20</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1380,7 +1385,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1394,7 +1399,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
@@ -1408,7 +1413,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
@@ -1422,7 +1427,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>80</v>
       </c>
@@ -1436,7 +1441,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1469,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>83</v>
       </c>
@@ -1478,7 +1483,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1492,7 +1497,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -1520,7 +1525,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -1534,7 +1539,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -1548,7 +1553,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1562,7 +1567,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>77</v>
       </c>
@@ -1590,7 +1595,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -1604,7 +1609,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -1618,7 +1623,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
nog meer analyse :(
</commit_message>
<xml_diff>
--- a/analyse tabel.xlsx
+++ b/analyse tabel.xlsx
@@ -798,9 +798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -994,16 +994,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1022,16 +1022,16 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1064,16 +1064,16 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1358,44 +1358,44 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B42" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Downgrade: Van java naar Processing.
</commit_message>
<xml_diff>
--- a/analyse tabel.xlsx
+++ b/analyse tabel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sijmen\Documents\SubSet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="6675" windowHeight="7230"/>
+    <workbookView xWindow="360" yWindow="72" windowWidth="6672" windowHeight="7236"/>
   </bookViews>
   <sheets>
     <sheet name="Functies" sheetId="2" r:id="rId1"/>
@@ -445,18 +450,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -471,12 +470,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -537,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +570,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -784,19 +782,20 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="201.28515625" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="201.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -810,801 +809,801 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B42" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B48" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>